<commit_message>
add: mail module add: graph module (unfinished) refactor: tweet_saver.py modified: other minor fixed
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IS2020-011\Documents\サイバーパトロール\tweet_saver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yamamotoo/Documents/archive/class_prB/webスクレイピング/完成github用/tweet_saver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB52F88-39AB-4D0D-9802-9E7CC5F109F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB5C49F-6700-F540-8B59-920821932512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="シート1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -317,47 +317,44 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1">
       <c r="A9" s="4"/>
     </row>
   </sheetData>

</xml_diff>